<commit_message>
Update sample projects to .NET 6
</commit_message>
<xml_diff>
--- a/SampleWebApp.Core/wwwroot/reports/report.xlsx
+++ b/SampleWebApp.Core/wwwroot/reports/report.xlsx
@@ -77,9 +77,9 @@
     <xf numFmtId="3" fontId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0"/>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="0" applyFont="1" xfId="1"/>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="0" applyFont="1" xfId="1" applyProtection="1"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,8 +112,8 @@
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.1919012069702" customWidth="1"/>
-    <col min="4" max="4" width="13.9526891708374" customWidth="1"/>
+    <col min="3" max="3" width="10.191901206970215" customWidth="1"/>
+    <col min="4" max="4" width="13.952689170837402" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>